<commit_message>
feat: Patent Researcher Swarm agent Draft v2.0
</commit_message>
<xml_diff>
--- a/src/PatentResearchSwarm.xlsx
+++ b/src/PatentResearchSwarm.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
   <si>
     <t>No</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Create Section Analysts</t>
   </si>
   <si>
-    <t>Human Feedback</t>
-  </si>
-  <si>
     <t>Conduct interview</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Download Data Collection on Google Patents</t>
   </si>
   <si>
-    <t>Assess the Patent Collection</t>
-  </si>
-  <si>
     <t>Data Analysis</t>
   </si>
   <si>
@@ -110,42 +104,18 @@
     <t>Technology cluster analysis</t>
   </si>
   <si>
-    <t>6.7.1</t>
-  </si>
-  <si>
-    <t>6.7.2</t>
-  </si>
-  <si>
-    <t>6.7.3</t>
-  </si>
-  <si>
-    <t>Select Source</t>
-  </si>
-  <si>
-    <t>6.7.4</t>
-  </si>
-  <si>
     <t>Search Data Subset Collection</t>
   </si>
   <si>
     <t>Search Descriptive Analytics Results</t>
   </si>
   <si>
-    <t>6.7.5</t>
-  </si>
-  <si>
     <t>Answer question</t>
   </si>
   <si>
-    <t>6.7.6</t>
-  </si>
-  <si>
     <t>Save Interview</t>
   </si>
   <si>
-    <t>6.7.7</t>
-  </si>
-  <si>
     <t>Write Section</t>
   </si>
   <si>
@@ -159,20 +129,6 @@
   </si>
   <si>
     <t>Consolidate Report</t>
-  </si>
-  <si>
-    <t>Finalize report</t>
-  </si>
-  <si>
-    <t>Render Report</t>
-  </si>
-  <si>
-    <t>1. Company Name &amp; Context: Organizational focus, existing portfolios, known R&amp;D efforts.
-2. Industry: Provides broad domain constraints (e.g., metallurgy, advanced materials, medical devices, cosmetics, electronics, energy, etc.).
-3. Products/Services: Clarifies whether you care about intermediate materials, final consumer products, or specialized equipment.
-4. Region: Pinpoints where you expect main market/competition (e.g., Asia, Europe, the Americas).
-5. Technology: The specific innovation angle (e.g., titanium extraction processes, Li-titanate electrodes, additive manufacturing of titanium alloys).
-6. Strategic Objectives: Are you seeking to (i) identify new processes, (ii) benchmark competitors, (iii) assess white spaces for R&amp;D, (iv) find licensing targets, etc.?</t>
   </si>
   <si>
     <t>1. Industry: Provides broad domain constraints (e.g., metallurgy, advanced materials, medical devices, cosmetics, electronics, energy, etc.).
@@ -181,47 +137,151 @@
 4. Research statement</t>
   </si>
   <si>
-    <t>1. Research Statement: A clear articulation of the research focus and objectives.
-2. High-Level Domain Research Map: An initial visual or conceptual map outlining the broad research domain.</t>
-  </si>
-  <si>
-    <t>1. Identification of Main Domains and Relationships: Recognizing interconnected domains and their relevance to the overall research focus.
-2. Foundation for Defining Research Sub-Fields: Establishing the groundwork for deeper segmentation.</t>
-  </si>
-  <si>
-    <t>1. High-Level Domain Research Map: From Process 1.
-2. Identification of Subdivision Dimensions: Core process, end-application, region, strategic angle.
+    <t>Consolidate sub research fields</t>
+  </si>
+  <si>
+    <t>1. Consolidate list of sub-field research</t>
+  </si>
+  <si>
+    <t>1. Company Name &amp; Context
+Type: String or Composite Object
+Definition:
+The full name of the company along with contextual information about its organizational focus, background, existing patent portfolios, and known research and development (R&amp;D) efforts.
+Example:
+"EcoBattery Inc. – A leader in sustainable battery technologies with a strong history in R&amp;D focused on advanced lithium‐titanate electrode development."
+2. Industry
+Type: String
+Definition:
+The broad market or economic sector in which the company operates. This provides domain constraints for the patent search.
+Example:
+"Energy Storage &amp; Battery Manufacturing"
+3. Products/Services
+Type: String or List of Strings
+Definition:
+A description of the company’s offerings. This variable indicates whether the focus is on intermediate materials (e.g., feedstocks), final consumer products, or specialized equipment.
+Example:
+"Advanced lithium-titanate battery electrodes"
+4. Region
+Type: String or List of Strings
+Definition:
+The geographic area(s) where the company primarily operates or faces competition. This variable helps target patent data by market.
+Example:
+"Global focus with emphasis on Asia and Europe"
+5. Technology
+Type: String or List of Strings
+Definition:
+The specific innovation or technical area that is the focus of the analysis. It may include processes, materials, or product-specific technology.
+Example:
+"Li-titanate electrode innovation, including advanced doping techniques and manufacturing methods."
+6. Strategic Objectives
+Type: List of Strings
+Definition:
+A set of clearly stated goals that drive the analysis. These objectives can include identifying new processes, benchmarking competitors, uncovering R&amp;D white spaces, or finding licensing opportunities.
+Example:
+["Identify new Li-titanate electrode processes", "Benchmark competitor technologies", "Assess potential R&amp;D white spaces", "Discover licensing targets"]</t>
+  </si>
+  <si>
+    <t>1. Research Statement
+Type: String
+Definition:
+A concise narrative that combines all input variables into a focused description of the research objective. It should capture the essence of the company’s strategic and technological goals.
+Example:
+"To map the patent landscape of advanced Li-titanate electrode technologies, emphasizing innovative doping and manufacturing techniques to identify emerging opportunities and benchmark global competitors."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. List of Main Domains &amp; Relationships
+Type: Structured List or JSON Object
+Definition:
+A detailed, structured breakdown of the high-level research domains along with descriptions of how these areas interrelate.
+Example:
+json
+Copiar
+[
+  { "domain": "Core Process", "elements": ["Doping Techniques", "Manufacturing Methods"], "relationship": "Innovation in doping directly affects electrode performance." },
+  { "domain": "End Application", "elements": ["EV Batteries", "Consumer Electronics"], "relationship": "Application requirements drive process innovation." }
+]
+</t>
+  </si>
+  <si>
+    <t>1. List of Main Domains &amp; Relationships
 3. Strategic Objectives: From Process 1.</t>
   </si>
   <si>
-    <t>1. List of Defined Research Sub-Fields: Specific areas within the broader domain to be explored.
-2. Structured Segmentation: Organized breakdown of the research domain into manageable and relevant sub-fields.</t>
-  </si>
-  <si>
-    <t>1. High-Level Domain Research Map: From Process 1.
-2. Identification of Subdivision Dimensions: Core process, end-application, region, strategic angle.</t>
-  </si>
-  <si>
-    <t>1. Specific Sub-Fields Based on Core Process/Technology Approach: E.g., Smelting &amp; Upgrading, Hydrometallurgical Processes.</t>
-  </si>
-  <si>
-    <t>1. High-Level Domain Research Map: From Process 1.
-2. Identification of Subdivision Dimensions: Core process, end-application, region, strategic angle.
-3. Company Products/Services Focus: Aligning sub-fields with company offerings.</t>
-  </si>
-  <si>
-    <t>1. Specific Sub-Fields Based on End-Application/Functional Use: E.g., Ceramics &amp; Electronic Components, Electrodes for Batteries.</t>
-  </si>
-  <si>
-    <t>1. High-Level Domain Research Map: From Process 1.
-2. Identification of Subdivision Dimensions: Core process, end-application, region, strategic angle.
-3. Company Strategic Objectives: From Process 1.</t>
-  </si>
-  <si>
-    <t>1. Specific Sub-Fields Based on Strategic/Competitive Angle: E.g., Key Competitor Portfolios, White Spaces for R&amp;D.</t>
-  </si>
-  <si>
-    <t>1. Defined Research Sub-Fields: From Process 3.
+    <t>1. List of Defined Research Sub-Fields
+Type: List or Array of Objects
+Definition:
+A catalog of distinct research segments that cover the overall domain. Each sub-field is named and described based on one or more of the subdivision dimensions.
+Example:
+["Smelting &amp; Upgrading", "Direct Acid Leaching Processes", "Battery Electrode Innovations", "China-Focused Technologies", "Key Competitor Portfolios"]</t>
+  </si>
+  <si>
+    <t>1. List of Defined Research Sub-Fields.
+2. Technology.
+3. Strategic Objectives</t>
+  </si>
+  <si>
+    <t>1. List of Defined Research Sub-Fields.
+2. Product/services
+3. Strategic Objectives</t>
+  </si>
+  <si>
+    <t>1. List of Defined Research Sub-Fields.
+2. Region.
+3. Strategic Objectives</t>
+  </si>
+  <si>
+    <t>1. List of Defined Research Sub-Fields.
+2. Strategic Objectives</t>
+  </si>
+  <si>
+    <t>1. Sub-Fields Based on Core Process/Technology
+Type: List of Strings or Objects
+Definition:
+A set of sub-fields defined exclusively by their technological process or method.
+Example:
+["Smelting &amp; Upgrading", "Innovative Hydrometallurgical Processes", "Advanced Electrolytic Reduction Methods"]</t>
+  </si>
+  <si>
+    <t>1. Sub-Fields Based on End-Applications
+Type: List of Strings or Objects
+Definition:
+A list of sub-fields categorized by their final functional use.
+Example:
+["Electrodes for Batteries", "Medical Device Applications", "Cosmetic Formulations"]</t>
+  </si>
+  <si>
+    <t>1. Sub-Fields Based on Regional Focus
+Type: List of Strings
+Definition:
+A list of sub-fields segmented by specific geographic or market focus.
+Example:
+["China-Focused Technologies", "US/EU Market Innovations"]</t>
+  </si>
+  <si>
+    <t>1. Sub-Fields Based on Strategic/Competitive Angle
+Type: List of Strings
+Definition:
+A set of sub-fields that capture strategic or competitive perspectives.
+Example:
+["Key Competitor Portfolios", "White Spaces for R&amp;D", "Collaboration Opportunities"]</t>
+  </si>
+  <si>
+    <t>1. Sub-Fields Based on Core Process/Technology.
+2. Sub-Fields Based on End-Applications.
+3. Sub-Fields Based on Regional Focus.
+4. Sub-Fields Based on Strategic/Competitive Angle</t>
+  </si>
+  <si>
+    <t>1. Prioritized Sub-Field List
+Type: List of Strings
+Definition:
+A list of sub-fields ranked by strategic importance and relevance.
+Example:
+["Battery Electrodes", "Emerging Green Technologies", "Key Competitor Portfolios"]</t>
+  </si>
+  <si>
+    <t>1. Consolidate list of sub-field research.
+2. Number of desired sub-fields.
 1. Company Name &amp; Context: Organizational focus, existing portfolios, known R&amp;D efforts.
 2. Industry: Provides broad domain constraints (e.g., metallurgy, advanced materials, medical devices, cosmetics, electronics, energy, etc.).
 3. Products/Services: Clarifies whether you care about intermediate materials, final consumer products, or specialized equipment.
@@ -230,30 +290,215 @@
 6. Strategic Objectives: Are you seeking to (i) identify new processes, (ii) benchmark competitors, (iii) assess white spaces for R&amp;D, (iv) find licensing targets, etc.?</t>
   </si>
   <si>
-    <t>1. Alignment of Each Sub-Field with Company Inputs: Ensuring each sub-field is relevant to strategic objectives.
-2. Identification of Relevant Sub-Fields for Deep-Dive: Prioritizing sub-fields based on strategic importance.</t>
-  </si>
-  <si>
-    <t>1. Defined Sub-Fields: From Process 3.
-2. Research Questions and Objectives per Sub-Field: Tailored inquiries for each area.</t>
-  </si>
-  <si>
-    <t>3. Assigned Researchers or Teams: Designated individuals or groups responsible for each sub-field.
-1. Detailed Research Plans for Each Sub-Field: Specific approaches and methodologies.
-2. Assigned Responsibilities and Tasks: Clear delegation of research activities.
-3. Structured Approach for Deep-Dive Research: Consistent and thorough investigation methods.</t>
-  </si>
-  <si>
-    <t>Consolidate sub research fields</t>
-  </si>
-  <si>
-    <t>1. Consolidate list of sub-field research</t>
-  </si>
-  <si>
-    <t>1. Specific Sub-Fields Based on Core Process/Technology Approach: E.g., Smelting &amp; Upgrading, Hydrometallurgical Processes.
-2. Specific Sub-Fields Based on Core Process/Technology Approach: E.g., Smelting &amp; Upgrading, Hydrometallurgical Processes.
-3. Specific Sub-Fields Based on End-Application/Functional Use: E.g., Ceramics &amp; Electronic Components, Electrodes for Batteries.
-4. Specific Sub-Fields Based on Strategic/Competitive Angle: E.g., Key Competitor Portfolios, White Spaces for R&amp;D.</t>
+    <t>1. Prioritized Sub-Field List</t>
+  </si>
+  <si>
+    <t>1. Research Plan for Sub-Field.
+Type: 
+jSON object
+Definition:
+A written plan outlining methodology, data sources, analysis techniques, and key questions for each sub-field.</t>
+  </si>
+  <si>
+    <t>1. Research Plan for Sub-Field.</t>
+  </si>
+  <si>
+    <t>1. Tailored Search Queries for Each Sub-Field
+Type: Query String or JSON Query Object
+Definition:
+Custom search equations that integrate all identified keywords, codes, and filters to retrieve the most relevant patents for each sub-field.
+Example:
+"((Li-titanate OR 'lithium titanate') AND (electrode OR battery)) AND (ICL: H01M-004) AND (EPRD &gt;= 2012)"</t>
+  </si>
+  <si>
+    <t>1. Tailored Search Queries for Each Sub-Field.</t>
+  </si>
+  <si>
+    <t>1. Retrieved Patent Documents per Sub-Field
+Type: Dataset/File (CSV, JSON, XML)
+Definition:
+A complete collection of patent documents downloaded based on the tailored search queries, stored in a structured data file.
+Example:
+A CSV file with columns for patent number, title, filing date, assignee, abstract, etc.
+2. Collected Data Sets for Analysis
+Type: Structured Data (DataFrame, JSON Object)
+Definition:
+The organized dataset ready for subsequent cleaning and analysis.
+Example:
+A pandas DataFrame containing the downloaded patent data.</t>
+  </si>
+  <si>
+    <t>1. Defined Relevance Criteria
+Type: List
+Definition:
+Specific rules to determine whether a patent is relevant to the sub-field (e.g., technological focus, filing date range).
+Example:
+"Include only patents that mention 'Li-titanate' in the title or abstract."
+2. Collected Data Sets for Analysis</t>
+  </si>
+  <si>
+    <t>Assess the Patent Collection (conditional edge)</t>
+  </si>
+  <si>
+    <t>1. Decision to continue or modifying the search equation.
+2. Rationale behind the assessment and suggestions (iff apply) for imporving future search equations.</t>
+  </si>
+  <si>
+    <t>1. Collected Data Sets for Analysis</t>
+  </si>
+  <si>
+    <t>1. Trend Analysis Data
+Type: Chart/Graph Object
+Definition:
+A visual or tabulated representation of how patent filings have changed over time. Patent number and Forward citations vs year.
+Example:
+A bar graph with filing counts per year.
+2. Growth Metrics
+Type: Numeric Value/Calculated Field
+Definition:
+Calculated values such as the Compound Annual Growth Rate (CAGR) or percentage increases.
+Example:
+"CAGR = 8.5%"
+3. Temporal Analysis of Patent Activity
+Type: Report/Data Table
+Definition:
+A detailed breakdown of patent activity trends, highlighting any seasonal or periodic fluctuations.
+Example:
+A table summarizing monthly filings for each year.
+4. Data Collection Subset (Top 5 cited patents per year, links)</t>
+  </si>
+  <si>
+    <t>1. List of Top Assignees/Filers per Sub-Field
+Type: Table/List/JSON
+Definition:
+A ranked list of the entities (companies, universities, institutions) that have filed the most patents in each sub-field.
+Example:
+A table with columns “Assignee”, “Patent Count”, “Market Share.”
+2. Competitive Landscape Insights
+Type: Report/JSON
+Definition:
+A qualitative and quantitative analysis that explains the dominance, filing strategies, and market influence of the key players.
+Example:
+A written section highlighting that “Samsung SDI leads in the battery electrodes sub-field with 35% market share.”
+3. Identification of Leading Companies and Institutions
+Type: List
+Definition:
+A curated list of the most influential organizations in the sub-field.
+Example:
+["Samsung SDI", "LG Chem", "MIT", "University of XYZ"]
+4. Data Collection Subset (Top 5 Cited patents in Top 5 Patent Assignee)</t>
+  </si>
+  <si>
+    <t>1. Technology Cluster Map
+Type: Diagram/Graph Object
+Definition:
+A visual representation (such as a network graph) that groups patents based on similar technological characteristics or shared keywords.
+Example:
+A network diagram showing clusters for “doping techniques” and “electrolytic reduction processes.”
+2. Cluster Insights Report
+Type: Document/JSON
+Definition:
+A report that details the characteristics, interrelations, and emerging trends within each identified technology cluster.
+Example:
+A summary noting that “a new cluster around green manufacturing is emerging with a 12% growth rate.”
+3. Data Collection Subset (Top 5 cited patents per Technology Cluster)</t>
+  </si>
+  <si>
+    <t>1. Research Template (from Process 6)
+2. Assignments of Sub-Fields to Analysts (Patent activity, key players, technology clusters)
+Type: List/Table
+Definition:
+A listing that assigns specific sub-fields to individual analysts or research teams based on expertise and workload.
+Example:
+{"Battery Electrodes": "Team A", "Green Doping Techniques": "Dr. Smith"}</t>
+  </si>
+  <si>
+    <t>1. List of Analyst Profiles</t>
+  </si>
+  <si>
+    <t>6.6.1</t>
+  </si>
+  <si>
+    <t>6.6.2</t>
+  </si>
+  <si>
+    <t>6.6.3</t>
+  </si>
+  <si>
+    <t>6.6.4</t>
+  </si>
+  <si>
+    <t>6.6.5</t>
+  </si>
+  <si>
+    <t>6.6.6</t>
+  </si>
+  <si>
+    <t>6.6.7</t>
+  </si>
+  <si>
+    <t>1. Analyst individual profile.
+2. Previous messages.</t>
+  </si>
+  <si>
+    <t>Search Web</t>
+  </si>
+  <si>
+    <t>1. Interview question: message</t>
+  </si>
+  <si>
+    <t>1. Context in the form of formatted docs</t>
+  </si>
+  <si>
+    <t>1. Analyst individual profile.
+2. Previous messages.
+3. Context in the form of formatted docs</t>
+  </si>
+  <si>
+    <t>1. Answer message</t>
+  </si>
+  <si>
+    <t>1. List of messages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Interview  </t>
+  </si>
+  <si>
+    <t>1. Analyst individual profile.
+2. Complete Interview
+3. Context in the form of formatted docs</t>
+  </si>
+  <si>
+    <t>1. Section Content (It could be Patent Activity, Key Players or Technology Clustering)</t>
+  </si>
+  <si>
+    <t>1. Industry: Provides broad domain constraints (e.g., metallurgy, advanced materials, medical devices, cosmetics, electronics, energy, etc.).
+2. Products/Services: Clarifies whether you care about intermediate materials, final consumer products, or specialized equipment.
+3. Technology: The specific innovation angle (e.g., titanium extraction processes, Li-titanate electrodes, additive manufacturing of titanium alloys).
+4. Research statement
+5. List of Sections</t>
+  </si>
+  <si>
+    <t>1. Conclusions.</t>
+  </si>
+  <si>
+    <t>1. Introduction.</t>
+  </si>
+  <si>
+    <t>1. Introduction.
+2. List of section content.
+3. Conclusions
+4. Images.
+5. jinja 2 templates for DocxTPL.</t>
+  </si>
+  <si>
+    <t>1. Rendered DOCX Sub-Field Report</t>
+  </si>
+  <si>
+    <t>1. Individual Rendered DOCX Sub-Field Reports</t>
+  </si>
+  <si>
+    <t>1. Consolidated Patent Research Landscape Report.</t>
   </si>
 </sst>
 </file>
@@ -583,19 +828,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="24.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="97.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -612,7 +859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -620,13 +867,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -634,13 +881,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -648,13 +895,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.1</v>
       </c>
@@ -662,13 +909,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.2</v>
       </c>
@@ -676,13 +923,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3.3</v>
       </c>
@@ -690,13 +937,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3.4</v>
       </c>
@@ -704,27 +951,27 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="270" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -732,13 +979,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -746,13 +993,13 @@
         <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -760,28 +1007,46 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>6.1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6.2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6.3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>20</v>
+        <v>61</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,42 +1054,66 @@
         <v>6.4</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="375" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="375" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="285" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6.5</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>6.6</v>
       </c>
@@ -832,117 +1121,163 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>6.7</v>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6.8</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>6.9</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>6.1</v>
+        <v>33</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>7</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>8</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>9</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Update state.py in each graph
</commit_message>
<xml_diff>
--- a/src/PatentResearchSwarm.xlsx
+++ b/src/PatentResearchSwarm.xlsx
@@ -13,7 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$32</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
   <si>
     <t>No</t>
   </si>
@@ -492,19 +496,117 @@
 5. jinja 2 templates for DocxTPL.</t>
   </si>
   <si>
-    <t>1. Rendered DOCX Sub-Field Report</t>
-  </si>
-  <si>
-    <t>1. Individual Rendered DOCX Sub-Field Reports</t>
-  </si>
-  <si>
-    <t>1. Consolidated Patent Research Landscape Report.</t>
+    <t>1. Consolidated Patent Research Landscape Report in DOCX</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>State variables</t>
+  </si>
+  <si>
+    <t>Patent Researcher Graph</t>
+  </si>
+  <si>
+    <t>Derive Sub-Field Graph</t>
+  </si>
+  <si>
+    <t>Sub-Field Research Graph</t>
+  </si>
+  <si>
+    <t>Data Analysis Graph</t>
+  </si>
+  <si>
+    <t>Conduct Interview Graph</t>
+  </si>
+  <si>
+    <t>Input State</t>
+  </si>
+  <si>
+    <t>Output State</t>
+  </si>
+  <si>
+    <t>1. Company Name &amp; Context
+2. Industry
+3. Products/Services
+4. Region
+5. Technology
+6. Strategic Objectives</t>
+  </si>
+  <si>
+    <t>1. Consolidated docx report directory string</t>
+  </si>
+  <si>
+    <t>1. List of Main Domains &amp; Relationships
+2. Strategic Objectives</t>
+  </si>
+  <si>
+    <t>1. Consolidated list of sub-fields for research</t>
+  </si>
+  <si>
+    <t>1. Consolidated list of sub-fields for research
+2. Number of desired sub-fields.</t>
+  </si>
+  <si>
+    <t>1. Prioritized List of Sub-Fields for research
+2. Research plan for each Sub-Field</t>
+  </si>
+  <si>
+    <t>1. List of strings with the individual DOCX report directories.
+2. jSON object with the str content for the different Sub-field patent-research report.</t>
+  </si>
+  <si>
+    <t>1. DOCX Sub-Field Patent research Report directory string</t>
+  </si>
+  <si>
+    <t>1. Patent activity jSON.
+1.1. Patent activity - Trend Analysis Graph PNG directory string
+1.2. Growth Metrics for Patent Activity
+1.3. Temporal Analysis Data of Patent Activity as string
+1.4. Data Collection Subset (Top 5 cited patents per year, links)
+2. Top Assignee jSON
+2.1. List of Top Assignees/Filers per Sub-Field Graph PNG directory string
+2.2. Top Assignees metrics.
+2.3. Identification of Leading Companies and Institutions
+2.4. Data Collection Subset (Top 5 Cited patents in Top 5 Patent Assignee patent links)
+3. Technology clusters JSON
+3.1. Technology Cluster Map Graph PNG directory string.
+3.2. List of technology clusters and definition.
+3.3. Data Collection Subset (Top 5 cited patents per Technology Cluster, patent link)</t>
+  </si>
+  <si>
+    <t>1. List of Analyst profiles.
+2. Patent activity jSON.
+3. Top Assignee jSON
+4. Technology clusters JSON</t>
+  </si>
+  <si>
+    <t>1. Collected Data Sets for Data Analysis per Sub-Field</t>
+  </si>
+  <si>
+    <t>1. Section Content (Should be Patent Activity, Key Players or Technology Clustering)
+2. List of Graph PNGs directory strings
+3. DOCX Sub-Field Patent research Report directory string</t>
+  </si>
+  <si>
+    <t>1. List of Rendered DOCX Sub-Field Report.
+2. List of jSON variables with report content.</t>
+  </si>
+  <si>
+    <t>1. Rendered DOCX Sub-Field Report
+2. jSON variable with report content per sub-field.</t>
+  </si>
+  <si>
+    <t>1. List of Rendered DOCX Sub-Field Reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,7 +647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -828,459 +930,721 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="D31:E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="97.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="8.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.1</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.2</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3.3</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3.4</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.5</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>6.1</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6.2</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6.3</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6.4</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="375" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="375" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="285" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="180" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6.5</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>6.6</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="75" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="135" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>6.7</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="180" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6.8</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>6.9</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="D32" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E32">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="6"/>
+        <filter val="6.1"/>
+        <filter val="6.2"/>
+        <filter val="6.3"/>
+        <filter val="6.4"/>
+        <filter val="6.5"/>
+        <filter val="6.6"/>
+        <filter val="6.7"/>
+        <filter val="6.8"/>
+        <filter val="6.90"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="3"/>
+    <col min="2" max="2" width="29.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="49.85546875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="360" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Including the creation of patent research sub-fields outline
</commit_message>
<xml_diff>
--- a/src/PatentResearchSwarm.xlsx
+++ b/src/PatentResearchSwarm.xlsx
@@ -931,7 +931,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7:E7"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +996,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3.1</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3.2</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3.3</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3.4</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.5</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>6.1</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6.2</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6.3</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6.4</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="180" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="180" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>6.5</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>6.6</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>6.7</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="180" hidden="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="180" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>6.8</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>6.9</v>
       </c>
@@ -1486,12 +1486,17 @@
   <autoFilter ref="A1:E32">
     <filterColumn colId="0">
       <filters>
-        <filter val="3"/>
-        <filter val="3.1"/>
-        <filter val="3.2"/>
-        <filter val="3.3"/>
-        <filter val="3.4"/>
-        <filter val="3.5"/>
+        <filter val="5"/>
+        <filter val="6"/>
+        <filter val="6.1"/>
+        <filter val="6.2"/>
+        <filter val="6.3"/>
+        <filter val="6.4"/>
+        <filter val="6.5"/>
+        <filter val="6.6"/>
+        <filter val="6.7"/>
+        <filter val="6.8"/>
+        <filter val="6.9"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>